<commit_message>
add updates from field work on 4/10/24
</commit_message>
<xml_diff>
--- a/data/TT24_phenology_dates.xlsx
+++ b/data/TT24_phenology_dates.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{322AC4EC-2D03-C442-8ED5-41B64F40BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A1B162-E671-B243-B98B-4C81C5ACF63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="500" windowWidth="42280" windowHeight="28040" xr2:uid="{4D8A3C15-14A0-044E-A149-F0D334F6D09B}"/>
+    <workbookView xWindow="1620" yWindow="500" windowWidth="45200" windowHeight="28300" xr2:uid="{4D8A3C15-14A0-044E-A149-F0D334F6D09B}"/>
   </bookViews>
   <sheets>
-    <sheet name="TRILLIUM" sheetId="1" r:id="rId1"/>
-    <sheet name="MAIANTHEMUM" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">TRILLIUM!$A$1:$L$105</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">TRILLIUM!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$187</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -132,6 +131,24 @@
   <si>
     <t>Tri</t>
   </si>
+  <si>
+    <t>untagged by between quad 2 and 4</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>4/10: some signs of chlorosis</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>orange flag</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
 </sst>
 </file>
 
@@ -153,15 +170,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -197,11 +220,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -216,49 +324,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -587,6 +688,44 @@
         </left>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -601,25 +740,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9865AAD-8F86-F54E-9FA0-1EE4DD1A7D38}" name="Table1" displayName="Table1" ref="A1:L105" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="14">
-  <autoFilter ref="A1:L105" xr:uid="{D9865AAD-8F86-F54E-9FA0-1EE4DD1A7D38}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9865AAD-8F86-F54E-9FA0-1EE4DD1A7D38}" name="Table1" displayName="Table1" ref="A1:L187" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:L187" xr:uid="{D9865AAD-8F86-F54E-9FA0-1EE4DD1A7D38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L105">
     <sortCondition ref="C2:C105"/>
     <sortCondition ref="A2:A105"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{4DD93A34-4A01-FE4A-90BA-5948ABB52889}" name="id" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{169BB96E-993D-E04D-BB8A-BE03C0BC36F9}" name="spp" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{25C0085E-768D-9347-86A9-5900797D647F}" name="plot" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{4C884772-B309-334D-994A-5F1917A74325}" name="subplot" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C87C6C52-FF2D-D840-ABC0-4D421484761E}" name="quadrat" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{CB7C6F01-8734-E240-9C89-F48CD097947D}" name="alive_23" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{F9DCBF60-B664-EE41-A9D8-ADD14E17AD5B}" name="abg_24" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{4254AC75-612F-7B46-A112-8E9C0ED38C1E}" name="date_unwhorled" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{DF0B242E-8913-4E4E-9AD5-3E3884A31C0D}" name="date_flowering" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{8A79CAFF-4477-AD42-BB22-C66A94CCDFEC}" name="date_senesce" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{9889C764-257E-C14C-94BE-415D9D7BAB52}" name="date_other" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{77FF84D2-ADA7-284F-ACD1-0DFFA49ADA16}" name="notes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4DD93A34-4A01-FE4A-90BA-5948ABB52889}" name="id" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{169BB96E-993D-E04D-BB8A-BE03C0BC36F9}" name="spp" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{25C0085E-768D-9347-86A9-5900797D647F}" name="plot" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4C884772-B309-334D-994A-5F1917A74325}" name="subplot" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{C87C6C52-FF2D-D840-ABC0-4D421484761E}" name="quadrat" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{CB7C6F01-8734-E240-9C89-F48CD097947D}" name="alive_23" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{F9DCBF60-B664-EE41-A9D8-ADD14E17AD5B}" name="abg_24" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{4254AC75-612F-7B46-A112-8E9C0ED38C1E}" name="date_unwhorled" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{DF0B242E-8913-4E4E-9AD5-3E3884A31C0D}" name="date_flowering" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{8A79CAFF-4477-AD42-BB22-C66A94CCDFEC}" name="date_senesce" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{9889C764-257E-C14C-94BE-415D9D7BAB52}" name="date_other" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{77FF84D2-ADA7-284F-ACD1-0DFFA49ADA16}" name="notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -945,10 +1084,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L187"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A113" zoomScale="110" zoomScaleNormal="280" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="J109" sqref="J109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,8 +1163,12 @@
       <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="7">
+        <v>45394</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -1050,8 +1193,12 @@
       <c r="F3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="7">
+        <v>45392</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1196,8 +1343,12 @@
       <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7">
+        <v>45392</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1222,7 +1373,9 @@
       <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1248,12 +1401,18 @@
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="7">
+        <v>45392</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -1274,7 +1433,9 @@
       <c r="F11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1300,8 +1461,12 @@
       <c r="F12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="7">
+        <v>45392</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1326,8 +1491,12 @@
       <c r="F13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="7">
+        <v>45392</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1355,7 +1524,9 @@
       <c r="G14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="7">
+        <v>45392</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1410,7 +1581,9 @@
       <c r="F16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1496,8 +1669,12 @@
       <c r="F19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="7">
+        <v>45392</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1552,8 +1729,12 @@
       <c r="F21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="7">
+        <v>45392</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1581,7 +1762,9 @@
       <c r="G22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="7">
+        <v>45392</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1606,8 +1789,12 @@
       <c r="F23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="3"/>
+      <c r="G23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7">
+        <v>45392</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1635,7 +1822,9 @@
       <c r="G24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="7">
+        <v>45392</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1663,7 +1852,9 @@
       <c r="G25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="7">
+        <v>45392</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1688,8 +1879,12 @@
       <c r="F26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="7">
+        <v>45392</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1714,8 +1909,12 @@
       <c r="F27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="3"/>
+      <c r="G27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="7">
+        <v>45392</v>
+      </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1740,8 +1939,12 @@
       <c r="F28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="7"/>
+      <c r="G28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="7">
+        <v>45392</v>
+      </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1769,7 +1972,9 @@
       <c r="G29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="3"/>
+      <c r="H29" s="7">
+        <v>45392</v>
+      </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1794,8 +1999,12 @@
       <c r="F30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="3"/>
+      <c r="G30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="7">
+        <v>45392</v>
+      </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1823,7 +2032,9 @@
       <c r="G31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" s="7">
+        <v>45392</v>
+      </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1848,12 +2059,18 @@
       <c r="F32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="7"/>
+      <c r="G32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="7">
+        <v>45392</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="5"/>
+      <c r="L32" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
@@ -1904,8 +2121,12 @@
       <c r="F34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="3"/>
+      <c r="G34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="7">
+        <v>45392</v>
+      </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -1933,7 +2154,9 @@
       <c r="G35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="7">
+        <v>45392</v>
+      </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -1961,7 +2184,9 @@
       <c r="G36" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="7">
+        <v>45392</v>
+      </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -1983,9 +2208,15 @@
       <c r="E37" s="4">
         <v>1</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="3"/>
+      <c r="F37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="7">
+        <v>45392</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2013,7 +2244,9 @@
       <c r="G38" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="3"/>
+      <c r="H38" s="7">
+        <v>45392</v>
+      </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2038,8 +2271,12 @@
       <c r="F39" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="3"/>
+      <c r="G39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="7">
+        <v>45392</v>
+      </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2067,7 +2304,9 @@
       <c r="G40" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="7">
+        <v>45392</v>
+      </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2095,7 +2334,9 @@
       <c r="G41" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="7">
+        <v>45392</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2125,7 +2366,9 @@
       <c r="G42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="7">
+        <v>45392</v>
+      </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2183,7 +2426,9 @@
       <c r="G44" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="7">
+        <v>45392</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2208,7 +2453,9 @@
       <c r="F45" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -2234,7 +2481,9 @@
       <c r="F46" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H46" s="7"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -2293,7 +2542,9 @@
       <c r="G48" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H48" s="3"/>
+      <c r="H48" s="7">
+        <v>45392</v>
+      </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -2320,7 +2571,9 @@
       <c r="F49" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G49" s="4"/>
+      <c r="G49" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
@@ -2349,7 +2602,9 @@
       <c r="G50" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H50" s="3"/>
+      <c r="H50" s="7">
+        <v>45392</v>
+      </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2377,7 +2632,9 @@
       <c r="G51" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H51" s="3"/>
+      <c r="H51" s="7">
+        <v>45392</v>
+      </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2405,7 +2662,9 @@
       <c r="G52" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H52" s="3"/>
+      <c r="H52" s="7">
+        <v>45392</v>
+      </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2433,11 +2692,15 @@
       <c r="G53" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H53" s="3"/>
+      <c r="H53" s="7">
+        <v>45392</v>
+      </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
-      <c r="L53" s="5"/>
+      <c r="L53" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="54" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
@@ -2458,8 +2721,12 @@
       <c r="F54" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G54" s="4"/>
-      <c r="H54" s="3"/>
+      <c r="G54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H54" s="7">
+        <v>45392</v>
+      </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2487,7 +2754,9 @@
       <c r="G55" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="7">
+        <v>45392</v>
+      </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2515,7 +2784,9 @@
       <c r="G56" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H56" s="3"/>
+      <c r="H56" s="7">
+        <v>45392</v>
+      </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -2540,7 +2811,9 @@
       <c r="F57" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H57" s="7">
         <v>45390</v>
       </c>
@@ -2571,7 +2844,9 @@
       <c r="G58" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H58" s="3"/>
+      <c r="H58" s="7">
+        <v>45392</v>
+      </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -2596,8 +2871,12 @@
       <c r="F59" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G59" s="4"/>
-      <c r="H59" s="3"/>
+      <c r="G59" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="7">
+        <v>45392</v>
+      </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -2622,8 +2901,12 @@
       <c r="F60" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G60" s="4"/>
-      <c r="H60" s="3"/>
+      <c r="G60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="7">
+        <v>45392</v>
+      </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -2648,12 +2931,18 @@
       <c r="F61" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G61" s="4"/>
-      <c r="H61" s="7"/>
+      <c r="G61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="7">
+        <v>45392</v>
+      </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="5"/>
+      <c r="L61" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="62" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
@@ -2674,8 +2963,12 @@
       <c r="F62" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="3"/>
+      <c r="G62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="7">
+        <v>45392</v>
+      </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -2700,8 +2993,12 @@
       <c r="F63" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="3"/>
+      <c r="G63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H63" s="7">
+        <v>45392</v>
+      </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -2789,7 +3086,9 @@
       <c r="G66" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H66" s="3"/>
+      <c r="H66" s="7">
+        <v>45392</v>
+      </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -2814,8 +3113,12 @@
       <c r="F67" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G67" s="4"/>
-      <c r="H67" s="3"/>
+      <c r="G67" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" s="7">
+        <v>45392</v>
+      </c>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -2902,7 +3205,9 @@
       <c r="F70" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G70" s="4"/>
+      <c r="G70" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
@@ -2930,8 +3235,12 @@
       <c r="F71" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G71" s="4"/>
-      <c r="H71" s="3"/>
+      <c r="G71" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H71" s="7">
+        <v>45392</v>
+      </c>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
@@ -2956,7 +3265,9 @@
       <c r="F72" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G72" s="4"/>
+      <c r="G72" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
@@ -2984,7 +3295,9 @@
       <c r="F73" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G73" s="4"/>
+      <c r="G73" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
@@ -3010,7 +3323,9 @@
       <c r="F74" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G74" s="4"/>
+      <c r="G74" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
@@ -3030,7 +3345,9 @@
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
+      <c r="G75" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
@@ -3056,7 +3373,9 @@
       <c r="F76" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G76" s="4"/>
+      <c r="G76" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
@@ -3082,8 +3401,12 @@
       <c r="F77" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G77" s="4"/>
-      <c r="H77" s="3"/>
+      <c r="G77" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H77" s="7">
+        <v>45392</v>
+      </c>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
@@ -3111,7 +3434,9 @@
       <c r="G78" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H78" s="3"/>
+      <c r="H78" s="7">
+        <v>45392</v>
+      </c>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
@@ -3136,8 +3461,12 @@
       <c r="F79" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G79" s="4"/>
-      <c r="H79" s="3"/>
+      <c r="G79" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H79" s="7">
+        <v>45392</v>
+      </c>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -3162,7 +3491,9 @@
       <c r="F80" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G80" s="4"/>
+      <c r="G80" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
@@ -3221,7 +3552,9 @@
       <c r="G82" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H82" s="3"/>
+      <c r="H82" s="7">
+        <v>45392</v>
+      </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -3246,7 +3579,9 @@
       <c r="F83" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G83" s="4"/>
+      <c r="G83" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
@@ -3272,8 +3607,12 @@
       <c r="F84" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G84" s="4"/>
-      <c r="H84" s="3"/>
+      <c r="G84" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H84" s="7">
+        <v>45392</v>
+      </c>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -3298,7 +3637,9 @@
       <c r="F85" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G85" s="4"/>
+      <c r="G85" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
@@ -3324,8 +3665,12 @@
       <c r="F86" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G86" s="4"/>
-      <c r="H86" s="3"/>
+      <c r="G86" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H86" s="7">
+        <v>45392</v>
+      </c>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -3350,7 +3695,9 @@
       <c r="F87" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H87" s="7"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
@@ -3379,7 +3726,9 @@
       <c r="G88" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H88" s="3"/>
+      <c r="H88" s="7">
+        <v>45392</v>
+      </c>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
@@ -3426,7 +3775,9 @@
       <c r="F90" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G90" s="4"/>
+      <c r="G90" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -3455,7 +3806,9 @@
       <c r="G91" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H91" s="3"/>
+      <c r="H91" s="7">
+        <v>45392</v>
+      </c>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -3480,8 +3833,12 @@
       <c r="F92" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G92" s="4"/>
-      <c r="H92" s="3"/>
+      <c r="G92" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H92" s="7">
+        <v>45392</v>
+      </c>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -3506,7 +3863,9 @@
       <c r="F93" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G93" s="4"/>
+      <c r="G93" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
@@ -3535,7 +3894,9 @@
       <c r="G94" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H94" s="3"/>
+      <c r="H94" s="7">
+        <v>45392</v>
+      </c>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
@@ -3560,7 +3921,9 @@
       <c r="F95" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G95" s="4"/>
+      <c r="G95" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
@@ -3589,7 +3952,9 @@
       <c r="G96" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H96" s="3"/>
+      <c r="H96" s="7">
+        <v>45392</v>
+      </c>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
@@ -3617,7 +3982,9 @@
       <c r="G97" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H97" s="3"/>
+      <c r="H97" s="7">
+        <v>45392</v>
+      </c>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
@@ -3642,7 +4009,9 @@
       <c r="F98" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G98" s="4"/>
+      <c r="G98" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
@@ -3668,7 +4037,9 @@
       <c r="F99" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G99" s="4"/>
+      <c r="G99" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
@@ -3697,7 +4068,9 @@
       <c r="G100" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H100" s="3"/>
+      <c r="H100" s="7">
+        <v>45392</v>
+      </c>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
@@ -3722,7 +4095,9 @@
       <c r="F101" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G101" s="4"/>
+      <c r="G101" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
@@ -3751,7 +4126,9 @@
       <c r="G102" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H102" s="3"/>
+      <c r="H102" s="7">
+        <v>45392</v>
+      </c>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
@@ -3776,12 +4153,16 @@
       <c r="F103" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G103" s="4"/>
+      <c r="G103" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
-      <c r="L103" s="5"/>
+      <c r="L103" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="104" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
@@ -3802,38 +4183,2172 @@
       <c r="F104" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G104" s="4"/>
+      <c r="G104" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
-      <c r="L104" s="5"/>
-    </row>
-    <row r="105" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C105" s="3">
-        <v>6</v>
-      </c>
-      <c r="D105" s="3">
+      <c r="L104" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="24">
+        <v>6</v>
+      </c>
+      <c r="D105" s="24">
         <v>5</v>
       </c>
-      <c r="E105" s="4">
+      <c r="E105" s="25">
         <v>4</v>
       </c>
-      <c r="F105" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G105" s="4"/>
-      <c r="H105" s="3"/>
-      <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="5"/>
+      <c r="F105" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G105" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+      <c r="J105" s="24"/>
+      <c r="K105" s="24"/>
+      <c r="L105" s="26"/>
+    </row>
+    <row r="106" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A106" s="18">
+        <v>4250</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C106" s="19">
+        <v>3</v>
+      </c>
+      <c r="D106" s="19">
+        <v>2</v>
+      </c>
+      <c r="E106" s="20">
+        <v>4</v>
+      </c>
+      <c r="F106" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G106" s="21"/>
+      <c r="H106" s="22"/>
+      <c r="I106" s="22"/>
+      <c r="J106" s="22"/>
+      <c r="K106" s="22"/>
+      <c r="L106" s="17"/>
+    </row>
+    <row r="107" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
+        <v>9412</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C107" s="3">
+        <v>3</v>
+      </c>
+      <c r="D107" s="3">
+        <v>3</v>
+      </c>
+      <c r="E107" s="4">
+        <v>1</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G107" s="4"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="17"/>
+    </row>
+    <row r="108" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A108" s="10">
+        <v>2310</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C108" s="8">
+        <v>3</v>
+      </c>
+      <c r="D108" s="8">
+        <v>4</v>
+      </c>
+      <c r="E108" s="9">
+        <v>2</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G108" s="4"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="17"/>
+    </row>
+    <row r="109" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>5105</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C109" s="3">
+        <v>3</v>
+      </c>
+      <c r="D109" s="3">
+        <v>8</v>
+      </c>
+      <c r="E109" s="4">
+        <v>3</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G109" s="4"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="17"/>
+    </row>
+    <row r="110" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A110" s="10">
+        <v>3643</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C110" s="8">
+        <v>3</v>
+      </c>
+      <c r="D110" s="8">
+        <v>12</v>
+      </c>
+      <c r="E110" s="9">
+        <v>2</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G110" s="4"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="17"/>
+    </row>
+    <row r="111" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>141</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C111" s="3">
+        <v>3</v>
+      </c>
+      <c r="D111" s="3">
+        <v>13</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G111" s="4"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="17"/>
+    </row>
+    <row r="112" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A112" s="10">
+        <v>5184</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C112" s="8">
+        <v>3</v>
+      </c>
+      <c r="D112" s="8">
+        <v>13</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G112" s="4"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="17"/>
+    </row>
+    <row r="113" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>54</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C113" s="3">
+        <v>3</v>
+      </c>
+      <c r="D113" s="3">
+        <v>16</v>
+      </c>
+      <c r="E113" s="4">
+        <v>4</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G113" s="4"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="17"/>
+    </row>
+    <row r="114" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A114" s="10">
+        <v>129</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="8">
+        <v>3</v>
+      </c>
+      <c r="D114" s="8">
+        <v>18</v>
+      </c>
+      <c r="E114" s="9">
+        <v>2</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G114" s="4"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="17"/>
+    </row>
+    <row r="115" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>2268</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C115" s="3">
+        <v>3</v>
+      </c>
+      <c r="D115" s="3">
+        <v>18</v>
+      </c>
+      <c r="E115" s="4">
+        <v>4</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G115" s="4"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="17"/>
+    </row>
+    <row r="116" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A116" s="10">
+        <v>6876</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C116" s="8">
+        <v>3</v>
+      </c>
+      <c r="D116" s="8">
+        <v>18</v>
+      </c>
+      <c r="E116" s="9">
+        <v>2</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G116" s="4"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="17"/>
+    </row>
+    <row r="117" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>6869</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C117" s="3">
+        <v>3</v>
+      </c>
+      <c r="D117" s="3">
+        <v>21</v>
+      </c>
+      <c r="E117" s="4">
+        <v>4</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G117" s="4"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+      <c r="L117" s="17"/>
+    </row>
+    <row r="118" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A118" s="10">
+        <v>2337</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" s="8">
+        <v>3</v>
+      </c>
+      <c r="D118" s="8">
+        <v>22</v>
+      </c>
+      <c r="E118" s="9">
+        <v>2</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G118" s="4"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="17"/>
+    </row>
+    <row r="119" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>1021</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C119" s="3">
+        <v>3</v>
+      </c>
+      <c r="D119" s="3">
+        <v>24</v>
+      </c>
+      <c r="E119" s="4">
+        <v>2</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" s="4"/>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+      <c r="L119" s="17"/>
+    </row>
+    <row r="120" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A120" s="10">
+        <v>5030</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C120" s="8">
+        <v>3</v>
+      </c>
+      <c r="D120" s="8">
+        <v>24</v>
+      </c>
+      <c r="E120" s="9">
+        <v>1</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G120" s="4"/>
+      <c r="H120" s="3"/>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="17"/>
+    </row>
+    <row r="121" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>5069</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="3">
+        <v>3</v>
+      </c>
+      <c r="D121" s="3">
+        <v>24</v>
+      </c>
+      <c r="E121" s="4">
+        <v>2</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G121" s="4"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="17"/>
+    </row>
+    <row r="122" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A122" s="14">
+        <v>179</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C122" s="15">
+        <v>3</v>
+      </c>
+      <c r="D122" s="15">
+        <v>30</v>
+      </c>
+      <c r="E122" s="16">
+        <v>2</v>
+      </c>
+      <c r="F122" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G122" s="13"/>
+      <c r="H122" s="12"/>
+      <c r="I122" s="12"/>
+      <c r="J122" s="12"/>
+      <c r="K122" s="12"/>
+      <c r="L122" s="17"/>
+    </row>
+    <row r="123" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>511</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C123" s="3">
+        <v>3</v>
+      </c>
+      <c r="D123" s="3">
+        <v>30</v>
+      </c>
+      <c r="E123" s="4">
+        <v>2</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G123" s="4"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="3"/>
+      <c r="K123" s="3"/>
+      <c r="L123" s="17"/>
+    </row>
+    <row r="124" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A124" s="10">
+        <v>543</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C124" s="8">
+        <v>3</v>
+      </c>
+      <c r="D124" s="8">
+        <v>30</v>
+      </c>
+      <c r="E124" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F124" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G124" s="4"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="17"/>
+    </row>
+    <row r="125" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>1157</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C125" s="3">
+        <v>3</v>
+      </c>
+      <c r="D125" s="3">
+        <v>30</v>
+      </c>
+      <c r="E125" s="4">
+        <v>1</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G125" s="4"/>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="3"/>
+      <c r="K125" s="3"/>
+      <c r="L125" s="17"/>
+    </row>
+    <row r="126" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A126" s="10">
+        <v>1663</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="8">
+        <v>3</v>
+      </c>
+      <c r="D126" s="8">
+        <v>30</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F126" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G126" s="4"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="17"/>
+    </row>
+    <row r="127" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>2131</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="3">
+        <v>3</v>
+      </c>
+      <c r="D127" s="3">
+        <v>30</v>
+      </c>
+      <c r="E127" s="4">
+        <v>2</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G127" s="4"/>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="3"/>
+      <c r="K127" s="3"/>
+      <c r="L127" s="17"/>
+    </row>
+    <row r="128" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A128" s="10">
+        <v>3665</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C128" s="8">
+        <v>3</v>
+      </c>
+      <c r="D128" s="8">
+        <v>30</v>
+      </c>
+      <c r="E128" s="9">
+        <v>1</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G128" s="4"/>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="17"/>
+    </row>
+    <row r="129" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>6900</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C129" s="3">
+        <v>5</v>
+      </c>
+      <c r="D129" s="3">
+        <v>2</v>
+      </c>
+      <c r="E129" s="4">
+        <v>4</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G129" s="4"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="3"/>
+      <c r="K129" s="3"/>
+      <c r="L129" s="17"/>
+    </row>
+    <row r="130" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A130" s="10">
+        <v>631</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130" s="8">
+        <v>5</v>
+      </c>
+      <c r="D130" s="8">
+        <v>3</v>
+      </c>
+      <c r="E130" s="9">
+        <v>3</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G130" s="4"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="17"/>
+    </row>
+    <row r="131" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>3960</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="3">
+        <v>5</v>
+      </c>
+      <c r="D131" s="3">
+        <v>3</v>
+      </c>
+      <c r="E131" s="4">
+        <v>1</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G131" s="4"/>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+      <c r="L131" s="17"/>
+    </row>
+    <row r="132" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A132" s="10">
+        <v>3993</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" s="8">
+        <v>5</v>
+      </c>
+      <c r="D132" s="8">
+        <v>3</v>
+      </c>
+      <c r="E132" s="9">
+        <v>1</v>
+      </c>
+      <c r="F132" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G132" s="4"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="17"/>
+    </row>
+    <row r="133" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C133" s="3">
+        <v>5</v>
+      </c>
+      <c r="D133" s="3">
+        <v>3</v>
+      </c>
+      <c r="E133" s="4">
+        <v>3</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G133" s="4"/>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="3"/>
+      <c r="K133" s="3"/>
+      <c r="L133" s="17"/>
+    </row>
+    <row r="134" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A134" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" s="8">
+        <v>5</v>
+      </c>
+      <c r="D134" s="8">
+        <v>3</v>
+      </c>
+      <c r="E134" s="9">
+        <v>3</v>
+      </c>
+      <c r="F134" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G134" s="4"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="17"/>
+    </row>
+    <row r="135" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>1432</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C135" s="3">
+        <v>5</v>
+      </c>
+      <c r="D135" s="3">
+        <v>17</v>
+      </c>
+      <c r="E135" s="4">
+        <v>2</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G135" s="4"/>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="17"/>
+    </row>
+    <row r="136" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A136" s="10">
+        <v>1499</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C136" s="8">
+        <v>5</v>
+      </c>
+      <c r="D136" s="8">
+        <v>17</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F136" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G136" s="4"/>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="17"/>
+    </row>
+    <row r="137" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>2803</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" s="3">
+        <v>5</v>
+      </c>
+      <c r="D137" s="3">
+        <v>18</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G137" s="4"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="17"/>
+    </row>
+    <row r="138" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A138" s="10">
+        <v>1476</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C138" s="8">
+        <v>5</v>
+      </c>
+      <c r="D138" s="8">
+        <v>23</v>
+      </c>
+      <c r="E138" s="9">
+        <v>1</v>
+      </c>
+      <c r="F138" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G138" s="4"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="17"/>
+    </row>
+    <row r="139" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>4781</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C139" s="3">
+        <v>5</v>
+      </c>
+      <c r="D139" s="3">
+        <v>23</v>
+      </c>
+      <c r="E139" s="4">
+        <v>1</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G139" s="4"/>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="3"/>
+      <c r="K139" s="3"/>
+      <c r="L139" s="17"/>
+    </row>
+    <row r="140" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A140" s="10">
+        <v>5657</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C140" s="8">
+        <v>5</v>
+      </c>
+      <c r="D140" s="8">
+        <v>23</v>
+      </c>
+      <c r="E140" s="9">
+        <v>1</v>
+      </c>
+      <c r="F140" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G140" s="4"/>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="17"/>
+    </row>
+    <row r="141" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>2616</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C141" s="3">
+        <v>5</v>
+      </c>
+      <c r="D141" s="3">
+        <v>36</v>
+      </c>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G141" s="4"/>
+      <c r="H141" s="3"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="3"/>
+      <c r="K141" s="3"/>
+      <c r="L141" s="17"/>
+    </row>
+    <row r="142" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A142" s="14">
+        <v>2637</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" s="15">
+        <v>5</v>
+      </c>
+      <c r="D142" s="15">
+        <v>36</v>
+      </c>
+      <c r="E142" s="16">
+        <v>3</v>
+      </c>
+      <c r="F142" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G142" s="13"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="12"/>
+      <c r="J142" s="12"/>
+      <c r="K142" s="12"/>
+      <c r="L142" s="17"/>
+    </row>
+    <row r="143" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>2662</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143" s="3">
+        <v>5</v>
+      </c>
+      <c r="D143" s="3">
+        <v>36</v>
+      </c>
+      <c r="E143" s="4">
+        <v>3</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G143" s="4"/>
+      <c r="H143" s="3"/>
+      <c r="I143" s="3"/>
+      <c r="J143" s="3"/>
+      <c r="K143" s="3"/>
+      <c r="L143" s="17"/>
+    </row>
+    <row r="144" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A144" s="10">
+        <v>5052</v>
+      </c>
+      <c r="B144" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="8">
+        <v>5</v>
+      </c>
+      <c r="D144" s="8">
+        <v>36</v>
+      </c>
+      <c r="E144" s="9">
+        <v>3</v>
+      </c>
+      <c r="F144" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G144" s="4"/>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="17"/>
+    </row>
+    <row r="145" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>5122</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="3">
+        <v>6</v>
+      </c>
+      <c r="D145" s="3">
+        <v>2</v>
+      </c>
+      <c r="E145" s="4">
+        <v>4</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G145" s="4"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="17"/>
+    </row>
+    <row r="146" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A146" s="10">
+        <v>1144</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="8">
+        <v>6</v>
+      </c>
+      <c r="D146" s="8">
+        <v>8</v>
+      </c>
+      <c r="E146" s="9">
+        <v>4</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G146" s="4"/>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="17"/>
+    </row>
+    <row r="147" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>1146</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C147" s="3">
+        <v>6</v>
+      </c>
+      <c r="D147" s="3">
+        <v>8</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G147" s="4"/>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="17"/>
+    </row>
+    <row r="148" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A148" s="10">
+        <v>1406</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C148" s="8">
+        <v>6</v>
+      </c>
+      <c r="D148" s="8">
+        <v>8</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F148" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G148" s="4"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="17"/>
+    </row>
+    <row r="149" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>1495</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C149" s="3">
+        <v>6</v>
+      </c>
+      <c r="D149" s="3">
+        <v>8</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G149" s="4"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="17"/>
+    </row>
+    <row r="150" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A150" s="10">
+        <v>3120</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C150" s="8">
+        <v>6</v>
+      </c>
+      <c r="D150" s="8">
+        <v>8</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G150" s="4"/>
+      <c r="H150" s="3"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="17"/>
+    </row>
+    <row r="151" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>4249</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C151" s="3">
+        <v>6</v>
+      </c>
+      <c r="D151" s="3">
+        <v>8</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F151" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G151" s="4"/>
+      <c r="H151" s="3"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="3"/>
+      <c r="K151" s="3"/>
+      <c r="L151" s="17"/>
+    </row>
+    <row r="152" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A152" s="10">
+        <v>4722</v>
+      </c>
+      <c r="B152" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C152" s="8">
+        <v>6</v>
+      </c>
+      <c r="D152" s="8">
+        <v>8</v>
+      </c>
+      <c r="E152" s="9">
+        <v>2</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G152" s="4"/>
+      <c r="H152" s="3"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+      <c r="L152" s="17"/>
+    </row>
+    <row r="153" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A153" s="2">
+        <v>5009</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C153" s="3">
+        <v>6</v>
+      </c>
+      <c r="D153" s="3">
+        <v>8</v>
+      </c>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G153" s="4"/>
+      <c r="H153" s="3"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="3"/>
+      <c r="K153" s="3"/>
+      <c r="L153" s="17"/>
+    </row>
+    <row r="154" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A154" s="10">
+        <v>5596</v>
+      </c>
+      <c r="B154" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C154" s="8">
+        <v>6</v>
+      </c>
+      <c r="D154" s="8">
+        <v>8</v>
+      </c>
+      <c r="E154" s="9">
+        <v>4</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G154" s="4"/>
+      <c r="H154" s="3"/>
+      <c r="I154" s="3"/>
+      <c r="J154" s="3"/>
+      <c r="K154" s="3"/>
+      <c r="L154" s="17"/>
+    </row>
+    <row r="155" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A155" s="2">
+        <v>3468</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C155" s="3">
+        <v>6</v>
+      </c>
+      <c r="D155" s="3">
+        <v>9</v>
+      </c>
+      <c r="E155" s="4">
+        <v>1</v>
+      </c>
+      <c r="F155" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G155" s="4"/>
+      <c r="H155" s="3"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="3"/>
+      <c r="K155" s="3"/>
+      <c r="L155" s="17"/>
+    </row>
+    <row r="156" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A156" s="10">
+        <v>5607</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C156" s="8">
+        <v>6</v>
+      </c>
+      <c r="D156" s="8">
+        <v>9</v>
+      </c>
+      <c r="E156" s="9">
+        <v>3</v>
+      </c>
+      <c r="F156" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G156" s="4"/>
+      <c r="H156" s="3"/>
+      <c r="I156" s="3"/>
+      <c r="J156" s="3"/>
+      <c r="K156" s="3"/>
+      <c r="L156" s="17"/>
+    </row>
+    <row r="157" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>5664</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C157" s="3">
+        <v>6</v>
+      </c>
+      <c r="D157" s="3">
+        <v>9</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G157" s="4"/>
+      <c r="H157" s="3"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="3"/>
+      <c r="K157" s="3"/>
+      <c r="L157" s="17"/>
+    </row>
+    <row r="158" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A158" s="10">
+        <v>3438</v>
+      </c>
+      <c r="B158" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C158" s="8">
+        <v>6</v>
+      </c>
+      <c r="D158" s="8">
+        <v>11</v>
+      </c>
+      <c r="E158" s="9">
+        <v>3</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G158" s="4"/>
+      <c r="H158" s="3"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="3"/>
+      <c r="K158" s="3"/>
+      <c r="L158" s="17"/>
+    </row>
+    <row r="159" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A159" s="2">
+        <v>4216</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C159" s="3">
+        <v>6</v>
+      </c>
+      <c r="D159" s="3">
+        <v>11</v>
+      </c>
+      <c r="E159" s="4">
+        <v>3</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G159" s="4"/>
+      <c r="H159" s="3"/>
+      <c r="I159" s="3"/>
+      <c r="J159" s="3"/>
+      <c r="K159" s="3"/>
+      <c r="L159" s="17"/>
+    </row>
+    <row r="160" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A160" s="10">
+        <v>5025</v>
+      </c>
+      <c r="B160" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C160" s="8">
+        <v>6</v>
+      </c>
+      <c r="D160" s="8">
+        <v>11</v>
+      </c>
+      <c r="E160" s="9">
+        <v>3</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G160" s="4"/>
+      <c r="H160" s="3"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="17"/>
+    </row>
+    <row r="161" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A161" s="2">
+        <v>5569</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C161" s="3">
+        <v>6</v>
+      </c>
+      <c r="D161" s="3">
+        <v>11</v>
+      </c>
+      <c r="E161" s="4">
+        <v>3</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G161" s="4"/>
+      <c r="H161" s="3"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="3"/>
+      <c r="K161" s="3"/>
+      <c r="L161" s="17"/>
+    </row>
+    <row r="162" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A162" s="10">
+        <v>2799</v>
+      </c>
+      <c r="B162" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C162" s="8">
+        <v>6</v>
+      </c>
+      <c r="D162" s="8">
+        <v>14</v>
+      </c>
+      <c r="E162" s="9">
+        <v>2</v>
+      </c>
+      <c r="F162" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G162" s="4"/>
+      <c r="H162" s="3"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="3"/>
+      <c r="K162" s="3"/>
+      <c r="L162" s="17"/>
+    </row>
+    <row r="163" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A163" s="2">
+        <v>1941</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C163" s="3">
+        <v>6</v>
+      </c>
+      <c r="D163" s="3">
+        <v>19</v>
+      </c>
+      <c r="E163" s="4">
+        <v>2</v>
+      </c>
+      <c r="F163" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G163" s="4"/>
+      <c r="H163" s="3"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="17"/>
+    </row>
+    <row r="164" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A164" s="14">
+        <v>6483</v>
+      </c>
+      <c r="B164" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C164" s="15">
+        <v>6</v>
+      </c>
+      <c r="D164" s="15">
+        <v>19</v>
+      </c>
+      <c r="E164" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F164" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G164" s="13"/>
+      <c r="H164" s="12"/>
+      <c r="I164" s="12"/>
+      <c r="J164" s="12"/>
+      <c r="K164" s="12"/>
+      <c r="L164" s="17"/>
+    </row>
+    <row r="165" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A165" s="2">
+        <v>6893</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C165" s="3">
+        <v>6</v>
+      </c>
+      <c r="D165" s="3">
+        <v>19</v>
+      </c>
+      <c r="E165" s="4">
+        <v>3</v>
+      </c>
+      <c r="F165" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G165" s="4"/>
+      <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="3"/>
+      <c r="K165" s="3"/>
+      <c r="L165" s="17"/>
+    </row>
+    <row r="166" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A166" s="10">
+        <v>2801</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C166" s="8">
+        <v>6</v>
+      </c>
+      <c r="D166" s="8">
+        <v>20</v>
+      </c>
+      <c r="E166" s="9">
+        <v>4</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G166" s="4"/>
+      <c r="H166" s="3"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+      <c r="L166" s="17"/>
+    </row>
+    <row r="167" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A167" s="2">
+        <v>2639</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C167" s="3">
+        <v>6</v>
+      </c>
+      <c r="D167" s="3">
+        <v>21</v>
+      </c>
+      <c r="E167" s="4">
+        <v>3</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G167" s="4"/>
+      <c r="H167" s="3"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="3"/>
+      <c r="K167" s="3"/>
+      <c r="L167" s="17"/>
+    </row>
+    <row r="168" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A168" s="10">
+        <v>2692</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C168" s="8">
+        <v>6</v>
+      </c>
+      <c r="D168" s="8">
+        <v>21</v>
+      </c>
+      <c r="E168" s="9">
+        <v>3</v>
+      </c>
+      <c r="F168" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G168" s="4"/>
+      <c r="H168" s="3"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="3"/>
+      <c r="K168" s="3"/>
+      <c r="L168" s="17"/>
+    </row>
+    <row r="169" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A169" s="2">
+        <v>5506</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C169" s="3">
+        <v>6</v>
+      </c>
+      <c r="D169" s="3">
+        <v>21</v>
+      </c>
+      <c r="E169" s="4">
+        <v>3</v>
+      </c>
+      <c r="F169" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G169" s="4"/>
+      <c r="H169" s="3"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="3"/>
+      <c r="K169" s="3"/>
+      <c r="L169" s="17"/>
+    </row>
+    <row r="170" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A170" s="10">
+        <v>2688</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C170" s="8">
+        <v>6</v>
+      </c>
+      <c r="D170" s="8">
+        <v>22</v>
+      </c>
+      <c r="E170" s="9">
+        <v>2</v>
+      </c>
+      <c r="F170" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G170" s="4"/>
+      <c r="H170" s="3"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="3"/>
+      <c r="K170" s="3"/>
+      <c r="L170" s="17"/>
+    </row>
+    <row r="171" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A171" s="2">
+        <v>3175</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C171" s="3">
+        <v>6</v>
+      </c>
+      <c r="D171" s="3">
+        <v>22</v>
+      </c>
+      <c r="E171" s="4">
+        <v>2</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G171" s="4"/>
+      <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="3"/>
+      <c r="K171" s="3"/>
+      <c r="L171" s="17"/>
+    </row>
+    <row r="172" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A172" s="10">
+        <v>5567</v>
+      </c>
+      <c r="B172" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C172" s="8">
+        <v>6</v>
+      </c>
+      <c r="D172" s="8">
+        <v>22</v>
+      </c>
+      <c r="E172" s="9">
+        <v>2</v>
+      </c>
+      <c r="F172" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G172" s="4"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="3"/>
+      <c r="K172" s="3"/>
+      <c r="L172" s="17"/>
+    </row>
+    <row r="173" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A173" s="2">
+        <v>6463</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C173" s="3">
+        <v>6</v>
+      </c>
+      <c r="D173" s="3">
+        <v>22</v>
+      </c>
+      <c r="E173" s="4">
+        <v>2</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G173" s="4"/>
+      <c r="H173" s="3"/>
+      <c r="I173" s="3"/>
+      <c r="J173" s="3"/>
+      <c r="K173" s="3"/>
+      <c r="L173" s="17"/>
+    </row>
+    <row r="174" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A174" s="10">
+        <v>2608</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C174" s="8">
+        <v>6</v>
+      </c>
+      <c r="D174" s="8">
+        <v>25</v>
+      </c>
+      <c r="E174" s="9">
+        <v>4</v>
+      </c>
+      <c r="F174" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G174" s="4"/>
+      <c r="H174" s="3"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="3"/>
+      <c r="K174" s="3"/>
+      <c r="L174" s="17"/>
+    </row>
+    <row r="175" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>5579</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C175" s="3">
+        <v>6</v>
+      </c>
+      <c r="D175" s="3">
+        <v>25</v>
+      </c>
+      <c r="E175" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F175" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G175" s="4"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="3"/>
+      <c r="K175" s="3"/>
+      <c r="L175" s="17"/>
+    </row>
+    <row r="176" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A176" s="10">
+        <v>6495</v>
+      </c>
+      <c r="B176" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C176" s="8">
+        <v>6</v>
+      </c>
+      <c r="D176" s="8">
+        <v>25</v>
+      </c>
+      <c r="E176" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F176" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G176" s="4"/>
+      <c r="H176" s="3"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="3"/>
+      <c r="K176" s="3"/>
+      <c r="L176" s="17"/>
+    </row>
+    <row r="177" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A177" s="2">
+        <v>5024</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C177" s="3">
+        <v>6</v>
+      </c>
+      <c r="D177" s="3">
+        <v>27</v>
+      </c>
+      <c r="E177" s="4">
+        <v>1</v>
+      </c>
+      <c r="F177" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G177" s="4"/>
+      <c r="H177" s="3"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="3"/>
+      <c r="K177" s="3"/>
+      <c r="L177" s="17"/>
+    </row>
+    <row r="178" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A178" s="10">
+        <v>2726</v>
+      </c>
+      <c r="B178" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C178" s="8">
+        <v>6</v>
+      </c>
+      <c r="D178" s="8">
+        <v>30</v>
+      </c>
+      <c r="E178" s="9">
+        <v>4</v>
+      </c>
+      <c r="F178" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G178" s="4"/>
+      <c r="H178" s="3"/>
+      <c r="I178" s="3"/>
+      <c r="J178" s="3"/>
+      <c r="K178" s="3"/>
+      <c r="L178" s="17"/>
+    </row>
+    <row r="179" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A179" s="2">
+        <v>3136</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C179" s="3">
+        <v>6</v>
+      </c>
+      <c r="D179" s="3">
+        <v>32</v>
+      </c>
+      <c r="E179" s="4">
+        <v>2</v>
+      </c>
+      <c r="F179" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G179" s="4"/>
+      <c r="H179" s="3"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="3"/>
+      <c r="K179" s="3"/>
+      <c r="L179" s="17"/>
+    </row>
+    <row r="180" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A180" s="10">
+        <v>4237</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C180" s="8">
+        <v>6</v>
+      </c>
+      <c r="D180" s="8">
+        <v>32</v>
+      </c>
+      <c r="E180" s="9">
+        <v>1</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G180" s="4"/>
+      <c r="H180" s="3"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="3"/>
+      <c r="K180" s="3"/>
+      <c r="L180" s="17"/>
+    </row>
+    <row r="181" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A181" s="2">
+        <v>5178</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C181" s="3">
+        <v>6</v>
+      </c>
+      <c r="D181" s="3">
+        <v>32</v>
+      </c>
+      <c r="E181" s="4">
+        <v>3</v>
+      </c>
+      <c r="F181" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G181" s="4"/>
+      <c r="H181" s="3"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="3"/>
+      <c r="K181" s="3"/>
+      <c r="L181" s="17"/>
+    </row>
+    <row r="182" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A182" s="10">
+        <v>5600</v>
+      </c>
+      <c r="B182" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C182" s="8">
+        <v>6</v>
+      </c>
+      <c r="D182" s="8">
+        <v>32</v>
+      </c>
+      <c r="E182" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F182" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G182" s="4"/>
+      <c r="H182" s="3"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="3"/>
+      <c r="K182" s="3"/>
+      <c r="L182" s="17"/>
+    </row>
+    <row r="183" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A183" s="2">
+        <v>1467</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C183" s="3">
+        <v>6</v>
+      </c>
+      <c r="D183" s="3">
+        <v>36</v>
+      </c>
+      <c r="E183" s="4">
+        <v>2</v>
+      </c>
+      <c r="F183" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G183" s="4"/>
+      <c r="H183" s="3"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="3"/>
+      <c r="K183" s="3"/>
+      <c r="L183" s="17"/>
+    </row>
+    <row r="184" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A184" s="10">
+        <v>2743</v>
+      </c>
+      <c r="B184" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C184" s="8">
+        <v>6</v>
+      </c>
+      <c r="D184" s="8">
+        <v>36</v>
+      </c>
+      <c r="E184" s="9">
+        <v>2</v>
+      </c>
+      <c r="F184" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G184" s="4"/>
+      <c r="H184" s="3"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="3"/>
+      <c r="K184" s="3"/>
+      <c r="L184" s="17"/>
+    </row>
+    <row r="185" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A185" s="2">
+        <v>5504</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C185" s="3">
+        <v>6</v>
+      </c>
+      <c r="D185" s="3">
+        <v>36</v>
+      </c>
+      <c r="E185" s="4">
+        <v>2</v>
+      </c>
+      <c r="F185" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G185" s="4"/>
+      <c r="H185" s="3"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="3"/>
+      <c r="K185" s="3"/>
+      <c r="L185" s="17"/>
+    </row>
+    <row r="186" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A186" s="10">
+        <v>6448</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C186" s="8">
+        <v>6</v>
+      </c>
+      <c r="D186" s="8">
+        <v>36</v>
+      </c>
+      <c r="E186" s="9">
+        <v>4</v>
+      </c>
+      <c r="F186" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G186" s="4"/>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="17"/>
+    </row>
+    <row r="187" spans="1:12" ht="22" x14ac:dyDescent="0.3">
+      <c r="A187" s="11">
+        <v>6462</v>
+      </c>
+      <c r="B187" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C187" s="12">
+        <v>6</v>
+      </c>
+      <c r="D187" s="12">
+        <v>36</v>
+      </c>
+      <c r="E187" s="13">
+        <v>4</v>
+      </c>
+      <c r="F187" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G187" s="13"/>
+      <c r="H187" s="12"/>
+      <c r="I187" s="12"/>
+      <c r="J187" s="12"/>
+      <c r="K187" s="12"/>
+      <c r="L187" s="17"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L105">
@@ -3841,30 +6356,17 @@
     <sortCondition ref="D2:D105"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" fitToHeight="3" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="46" fitToHeight="3" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;"Aptos Narrow (Body),Bold"&amp;18 2024 TRILLIUM TRAIL PHENOLOGY
 DATASHEET (for carbon budgets)
 </oddHeader>
     <oddFooter>&amp;L&amp;"Aptos Narrow (Body),Regular"&amp;8unwhorled = first date of leaf unfolding w/ laminar surface exposed
 flowering = first date of open flower
-scenescence = leaves brown, chlorophyll content below detection, unstable photosynthesis (A &lt; 1)</oddFooter>
+senescence = leaves brown, chlorophyll content below detection, unstable photosynthesis (A&amp;Ynet&amp;Y &lt; 1)</oddFooter>
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40147251-3CE2-4B45-B3BD-A88F06F7C0B4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>